<commit_message>
Updated data and script
</commit_message>
<xml_diff>
--- a/keyboard.xlsx
+++ b/keyboard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\turtl\Documents\Classes\Spring 2023\STAT 4204\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\turtl\Documents\Classes\Spring 2023\STAT 4204\project\stat4204_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB98AABA-8414-4EA6-8F98-D51F7F51233D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CC5801-7370-495A-B475-8D15C1278799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFECF9C8-13B2-4552-AEA9-C09A49AF8F15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="7">
   <si>
     <t>Operator</t>
   </si>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1BEC98-7EC0-4937-8202-92F9C89F6485}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,6 +561,258 @@
         <v>98</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating names for keyboard types
</commit_message>
<xml_diff>
--- a/keyboard.xlsx
+++ b/keyboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\turtl\Documents\Classes\Spring 2023\STAT 4204\project\stat4204_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CC5801-7370-495A-B475-8D15C1278799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7DFCEB-0EFD-4495-918C-59B1B64804AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFECF9C8-13B2-4552-AEA9-C09A49AF8F15}"/>
   </bookViews>
@@ -44,19 +44,19 @@
     <t>Keyboard Type</t>
   </si>
   <si>
-    <t>Rubber Dome</t>
-  </si>
-  <si>
     <t>Typing Speed</t>
-  </si>
-  <si>
-    <t>Membrane</t>
   </si>
   <si>
     <t>Mechanical</t>
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>Dome-Switch</t>
+  </si>
+  <si>
+    <t>Scissor-Switch</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1BEC98-7EC0-4937-8202-92F9C89F6485}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -426,13 +426,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -443,7 +443,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>69</v>
@@ -457,7 +457,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>81</v>
@@ -471,7 +471,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>73</v>
@@ -485,7 +485,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>76</v>
@@ -499,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>83</v>
@@ -513,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <v>84</v>
@@ -527,7 +527,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8">
         <v>97</v>
@@ -541,7 +541,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>99</v>
@@ -555,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>98</v>
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>75</v>
@@ -583,7 +583,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D12">
         <v>86</v>
@@ -597,7 +597,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>83</v>
@@ -611,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>74</v>
@@ -625,7 +625,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>85</v>
@@ -639,7 +639,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D16">
         <v>80</v>
@@ -653,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>97</v>
@@ -667,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>98</v>
@@ -681,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>103</v>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>84</v>
@@ -709,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D21">
         <v>72</v>
@@ -723,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>83</v>
@@ -737,7 +737,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D23">
         <v>69</v>
@@ -751,7 +751,7 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>76</v>
@@ -765,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25">
         <v>87</v>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D26">
         <v>100</v>
@@ -793,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>88</v>
@@ -807,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D28">
         <v>96</v>

</xml_diff>